<commit_message>
main now correctly reads from files
</commit_message>
<xml_diff>
--- a/DATA/mtas.xlsx
+++ b/DATA/mtas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grovecitycollege-my.sharepoint.com/personal/graybillkb20_gcc_edu/Documents/Junior Year/COMP445A/ResearchProject/Code/DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grovecitycollege-my.sharepoint.com/personal/harmonsc21_gcc_edu/Documents/Jr_Spring/AI/Research_Project/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC10480B599968E05BDE58FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F28253BC-F49D-4EAC-8014-7A0169610CE0}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mtas" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,17 +404,17 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -442,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -456,7 +456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
started restricting domains. still in progress
</commit_message>
<xml_diff>
--- a/DATA/mtas.xlsx
+++ b/DATA/mtas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grovecitycollege-my.sharepoint.com/personal/harmonsc21_gcc_edu/Documents/Jr_Spring/AI/Research_Project/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC10480B599968E05BDE58FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F28253BC-F49D-4EAC-8014-7A0169610CE0}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC10480B599968E05BDE58FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0529C38-7D65-4925-BA01-1E0EC5BB977D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Type</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Rendition of Behold Our God</t>
+  </si>
+  <si>
+    <t>Rendition of Test</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +473,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added comments and improved readability. Implemented working version of backtrack
</commit_message>
<xml_diff>
--- a/DATA/mtas.xlsx
+++ b/DATA/mtas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grovecitycollege-my.sharepoint.com/personal/harmonsc21_gcc_edu/Documents/Jr_Spring/AI/Research_Project/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC10480B599968E05BDE58FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0529C38-7D65-4925-BA01-1E0EC5BB977D}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC10480B599968E05BDE58FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB5CDECF-715E-4081-AB1B-F9356FEC6627}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Type</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Rendition of Test</t>
+  </si>
+  <si>
+    <t>Drew Smith</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +481,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>30</v>

</xml_diff>

<commit_message>
added readme and main to MTA_Solver
</commit_message>
<xml_diff>
--- a/DATA/mtas.xlsx
+++ b/DATA/mtas.xlsx
@@ -1,81 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="mtas" sheetId="1" r:id="rId1"/>
+    <sheet name="mtas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Students</t>
-  </si>
-  <si>
-    <t>Length (minutes)</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Apologetics</t>
-  </si>
-  <si>
-    <t>Drama</t>
-  </si>
-  <si>
-    <t>Elizabeth Vaughn, Patricia Stewart</t>
-  </si>
-  <si>
-    <t>Frank Phillips</t>
-  </si>
-  <si>
-    <t>Brenda Jackson</t>
-  </si>
-  <si>
-    <t>MTA 1</t>
-  </si>
-  <si>
-    <t>MTA 2</t>
-  </si>
-  <si>
-    <t>MTA 3</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -406,70 +420,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Length (minutes)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Music</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pam Potts, Catherine Young</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>MTA 1</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Preaching</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pam Potts</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MTA 2</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>